<commit_message>
Add table extraction logic with scroll
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\pomanda demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FC7548-0833-4311-9C08-40551EA63829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59306454-6603-4180-B66F-97008FB0068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,9 +156,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>PomadaDemo</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>https://pomanda.com/</t>
+  </si>
+  <si>
+    <t>pomada</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -600,7 +600,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -621,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -629,18 +629,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add companies to queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\pomanda demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59306454-6603-4180-B66F-97008FB0068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496EA1F7-9801-4765-AECD-CFB5C6461251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>pomada</t>
+  </si>
+  <si>
+    <t>MaxExtractionCount</t>
+  </si>
+  <si>
+    <t>Max number of companies that can be extracted from the table every transaction</t>
+  </si>
+  <si>
+    <t>RetryNumberBulkAddQueueItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Bulk Add Queue Item activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
 </sst>
 </file>
@@ -549,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -643,7 +655,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1645,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1815,7 +1837,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Write company details to excel and fixing selectors
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\pomanda demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496EA1F7-9801-4765-AECD-CFB5C6461251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F0D1CF-0097-4886-8A08-468232FBED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -660,7 +660,7 @@
         <v>49</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -1667,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Add company detail:  phone number Fix writing to excel headers
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\pomanda demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F0D1CF-0097-4886-8A08-468232FBED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CFB77A-B021-4488-991C-CE87440AF9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="3375" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,160 +30,184 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OrchestratorQueueName</t>
+    </r>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>pomada</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
+    </r>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>PomadaDemo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+    </r>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>PomadaMainURL</t>
+  </si>
+  <si>
+    <t>https://pomanda.com/</t>
+  </si>
+  <si>
+    <t>PomadaSearchAllURL</t>
+  </si>
+  <si>
+    <t>https://pomanda.com/powersearch/company</t>
+  </si>
+  <si>
+    <t>MaxExtractionCount</t>
+  </si>
+  <si>
+    <t>Max number of companies that can be extracted from the table every transaction</t>
+  </si>
+  <si>
+    <t>MaxRetryNumber</t>
+  </si>
+  <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>RetryNumberBulkAddQueueItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Bulk Add Queue Item activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
     <t>Asset</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>OrchestratorAssetFolder</t>
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>System exception.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>PomadaDemo</t>
-  </si>
-  <si>
-    <t>PomadaSearchAllURL</t>
-  </si>
-  <si>
-    <t>PomadaMainURL</t>
-  </si>
-  <si>
-    <t>https://pomanda.com/powersearch/company</t>
-  </si>
-  <si>
-    <t>https://pomanda.com/</t>
-  </si>
-  <si>
-    <t>pomada</t>
-  </si>
-  <si>
-    <t>MaxExtractionCount</t>
-  </si>
-  <si>
-    <t>Max number of companies that can be extracted from the table every transaction</t>
-  </si>
-  <si>
-    <t>RetryNumberBulkAddQueueItem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Bulk Add Queue Item activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
 </sst>
 </file>
@@ -235,14 +259,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -561,11 +581,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -581,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -608,62 +628,61 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
+    <row r="3" spans="1:26" ht="45" customHeight="1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="30" customHeight="1">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1668,10 +1687,10 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1 A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1687,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1713,150 +1732,150 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="30" customHeight="1">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="45" customHeight="1">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="45" customHeight="1">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2840,9 +2859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -2855,13 +2874,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>

<commit_message>
Move Add Queue logic to initial state Change Bulk Add to single Add Queue Add reference to transaction items Add Unique queue logic Minor Fixes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENDI\Documents\UiPath\pomanda demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CFB77A-B021-4488-991C-CE87440AF9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548CB93A-F3CD-4755-B58C-FB4DAFFEC2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="3375" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -679,7 +679,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -2859,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>